<commit_message>
Update 22 JULI - 27  JULI 2024.xlsx
</commit_message>
<xml_diff>
--- a/STOCK UTN/22 JULI - 27  JULI 2024.xlsx
+++ b/STOCK UTN/22 JULI - 27  JULI 2024.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5804F3-EF37-44DA-B4F2-0A108A2ABB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="10530" windowHeight="10905" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JK KENKO" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">IMPORT!$A$2:$C$875</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'JK KENKO'!$A$85:$C$182</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -10768,7 +10769,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -10948,9 +10949,9 @@
   <cellStyles count="5">
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="常规 2" xfId="3"/>
-    <cellStyle name="常规 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="常规 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="常规 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -10985,7 +10986,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="Table Style 1" pivot="0" count="0"/>
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -10999,9 +11000,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -11039,9 +11040,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11076,7 +11077,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11111,7 +11112,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -11284,12 +11285,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A70" zoomScale="70" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A82" zoomScale="70" zoomScaleNormal="130" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
@@ -13470,17 +13471,17 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A81:C115">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A81:C115">
     <sortCondition ref="A80"/>
   </sortState>
+  <conditionalFormatting sqref="A1:A84">
+    <cfRule type="duplicateValues" dxfId="2" priority="160"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A84">
-    <cfRule type="duplicateValues" dxfId="0" priority="160"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.98425196850393704" right="0.39370078740157483" top="0.39370078740157483" bottom="1.6071428571428572" header="0.39370078740157483" footer="0.39370078740157483"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
@@ -13492,7 +13493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2096"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A2073" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
@@ -36822,11 +36823,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D960"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A935" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="A944" sqref="A944"/>
     </sheetView>
   </sheetViews>
@@ -50523,7 +50524,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D1004">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1004">
     <sortCondition ref="A2:A1004"/>
   </sortState>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="1.4173228346456694" header="0.39370078740157483" footer="0.19685039370078741"/>

</xml_diff>